<commit_message>
commented all code, correct output, runs in 83 seconds
</commit_message>
<xml_diff>
--- a/px_stats.xlsx
+++ b/px_stats.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD" numFmtId="165"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -16138,257 +16138,257 @@
     </row>
     <row r="986">
       <c r="A986" s="2" t="n">
-        <v>38078</v>
+        <v>38916</v>
       </c>
       <c r="B986" s="2" t="n">
-        <v>38106</v>
+        <v>38944</v>
       </c>
       <c r="C986" t="n">
         <v>29</v>
       </c>
       <c r="D986" t="inlineStr">
         <is>
-          <t>BBG002SD5BZ8</t>
+          <t>BBG000BB3S61</t>
         </is>
       </c>
     </row>
     <row r="987">
       <c r="A987" s="2" t="n">
-        <v>39692</v>
+        <v>38412</v>
       </c>
       <c r="B987" s="2" t="n">
-        <v>39720</v>
+        <v>38440</v>
       </c>
       <c r="C987" t="n">
         <v>29</v>
       </c>
       <c r="D987" t="inlineStr">
         <is>
-          <t>BBG002SD5BZ8</t>
+          <t>BBG000BCYCD2</t>
         </is>
       </c>
     </row>
     <row r="988">
       <c r="A988" s="2" t="n">
-        <v>39753</v>
+        <v>38504</v>
       </c>
       <c r="B988" s="2" t="n">
-        <v>39781</v>
+        <v>38532</v>
       </c>
       <c r="C988" t="n">
         <v>29</v>
       </c>
       <c r="D988" t="inlineStr">
         <is>
-          <t>BBG002SD5BZ8</t>
+          <t>BBG000BCYCD2</t>
         </is>
       </c>
     </row>
     <row r="989">
       <c r="A989" s="2" t="n">
-        <v>40330</v>
+        <v>42605</v>
       </c>
       <c r="B989" s="2" t="n">
-        <v>40358</v>
+        <v>42633</v>
       </c>
       <c r="C989" t="n">
         <v>29</v>
       </c>
       <c r="D989" t="inlineStr">
         <is>
-          <t>BBG002SD5BZ8</t>
+          <t>BBG000BDCP09</t>
         </is>
       </c>
     </row>
     <row r="990">
       <c r="A990" s="2" t="n">
-        <v>41365</v>
+        <v>39665</v>
       </c>
       <c r="B990" s="2" t="n">
-        <v>41393</v>
+        <v>39693</v>
       </c>
       <c r="C990" t="n">
         <v>29</v>
       </c>
       <c r="D990" t="inlineStr">
         <is>
-          <t>BBG002SD5BZ8</t>
+          <t>BBG000BDWWY5</t>
         </is>
       </c>
     </row>
     <row r="991">
       <c r="A991" s="2" t="n">
-        <v>37408</v>
+        <v>41193</v>
       </c>
       <c r="B991" s="2" t="n">
-        <v>37436</v>
+        <v>41221</v>
       </c>
       <c r="C991" t="n">
         <v>29</v>
       </c>
       <c r="D991" t="inlineStr">
         <is>
-          <t>BBG002SFJ3P7</t>
+          <t>BBG000BDWWY5</t>
         </is>
       </c>
     </row>
     <row r="992">
       <c r="A992" s="2" t="n">
-        <v>38961</v>
+        <v>41227</v>
       </c>
       <c r="B992" s="2" t="n">
-        <v>38989</v>
+        <v>41255</v>
       </c>
       <c r="C992" t="n">
         <v>29</v>
       </c>
       <c r="D992" t="inlineStr">
         <is>
-          <t>BBG002SFJ3P7</t>
+          <t>BBG000BDWWY5</t>
         </is>
       </c>
     </row>
     <row r="993">
       <c r="A993" s="2" t="n">
-        <v>39965</v>
+        <v>38469</v>
       </c>
       <c r="B993" s="2" t="n">
-        <v>39993</v>
+        <v>38497</v>
       </c>
       <c r="C993" t="n">
         <v>29</v>
       </c>
       <c r="D993" t="inlineStr">
         <is>
-          <t>BBG002SFJ3P7</t>
+          <t>BBG000BNHRC5</t>
         </is>
       </c>
     </row>
     <row r="994">
       <c r="A994" s="2" t="n">
-        <v>41426</v>
+        <v>39211</v>
       </c>
       <c r="B994" s="2" t="n">
-        <v>41454</v>
+        <v>39239</v>
       </c>
       <c r="C994" t="n">
         <v>29</v>
       </c>
       <c r="D994" t="inlineStr">
         <is>
-          <t>BBG002SFJ3P7</t>
+          <t>BBG000C1CK87</t>
         </is>
       </c>
     </row>
     <row r="995">
       <c r="A995" s="2" t="n">
-        <v>42887</v>
+        <v>37266</v>
       </c>
       <c r="B995" s="2" t="n">
-        <v>42915</v>
+        <v>37294</v>
       </c>
       <c r="C995" t="n">
         <v>29</v>
       </c>
       <c r="D995" t="inlineStr">
         <is>
-          <t>BBG002SFJ3P7</t>
+          <t>BBG000DGFSY4</t>
         </is>
       </c>
     </row>
     <row r="996">
       <c r="A996" s="2" t="n">
-        <v>38231</v>
+        <v>40673</v>
       </c>
       <c r="B996" s="2" t="n">
-        <v>38259</v>
+        <v>40701</v>
       </c>
       <c r="C996" t="n">
         <v>29</v>
       </c>
       <c r="D996" t="inlineStr">
         <is>
-          <t>BBG002SFKD19</t>
+          <t>BBG000F5YYN4</t>
         </is>
       </c>
     </row>
     <row r="997">
       <c r="A997" s="2" t="n">
-        <v>39753</v>
+        <v>39295</v>
       </c>
       <c r="B997" s="2" t="n">
-        <v>39781</v>
+        <v>39323</v>
       </c>
       <c r="C997" t="n">
         <v>29</v>
       </c>
       <c r="D997" t="inlineStr">
         <is>
-          <t>BBG002SFKD19</t>
+          <t>BBG000H11ST4</t>
         </is>
       </c>
     </row>
     <row r="998">
       <c r="A998" s="2" t="n">
-        <v>40634</v>
+        <v>40248</v>
       </c>
       <c r="B998" s="2" t="n">
-        <v>40662</v>
+        <v>40276</v>
       </c>
       <c r="C998" t="n">
         <v>29</v>
       </c>
       <c r="D998" t="inlineStr">
         <is>
-          <t>BBG002SFKD19</t>
+          <t>BBG000H11ST4</t>
         </is>
       </c>
     </row>
     <row r="999">
       <c r="A999" s="2" t="n">
-        <v>43252</v>
+        <v>39022</v>
       </c>
       <c r="B999" s="2" t="n">
-        <v>43280</v>
+        <v>39050</v>
       </c>
       <c r="C999" t="n">
         <v>29</v>
       </c>
       <c r="D999" t="inlineStr">
         <is>
-          <t>BBG002SFKD19</t>
+          <t>BBG000N6JH48</t>
         </is>
       </c>
     </row>
     <row r="1000">
       <c r="A1000" s="2" t="n">
-        <v>40269</v>
+        <v>37754</v>
       </c>
       <c r="B1000" s="2" t="n">
-        <v>40297</v>
+        <v>37782</v>
       </c>
       <c r="C1000" t="n">
         <v>29</v>
       </c>
       <c r="D1000" t="inlineStr">
         <is>
-          <t>BBG002SR11R2</t>
+          <t>BBG000NXBLD8</t>
         </is>
       </c>
     </row>
     <row r="1001">
       <c r="A1001" s="2" t="n">
-        <v>40787</v>
+        <v>38168</v>
       </c>
       <c r="B1001" s="2" t="n">
-        <v>40815</v>
+        <v>38196</v>
       </c>
       <c r="C1001" t="n">
         <v>29</v>
       </c>
       <c r="D1001" t="inlineStr">
         <is>
-          <t>BBG002SR11R2</t>
+          <t>BBG000NXBLD8</t>
         </is>
       </c>
     </row>

</xml_diff>